<commit_message>
Started test for CANID - skipped, not complete
</commit_message>
<xml_diff>
--- a/Documents/Supported Opcodes.xlsx
+++ b/Documents/Supported Opcodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\source\repos\David284\CbusTestSuite\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3370E7A1-572D-4E42-9191-D7C704669417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1A35DB-9666-4C59-8969-96566FDFBEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20760" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CANACC5" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
   <si>
     <t>WRACK</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>ERR</t>
+  </si>
+  <si>
+    <t>Runs bootloader</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
   </si>
 </sst>
 </file>
@@ -534,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +549,7 @@
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="5" max="5" width="11.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
@@ -599,6 +605,9 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -606,6 +615,9 @@
       </c>
       <c r="C7" t="s">
         <v>52</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrected '6F' as 'CMDERR'
</commit_message>
<xml_diff>
--- a/Documents/Supported Opcodes.xlsx
+++ b/Documents/Supported Opcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\source\repos\David284\CbusTestSuite\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1A35DB-9666-4C59-8969-96566FDFBEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42D94A6-193C-475D-9201-74A223F50DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -541,7 +541,7 @@
   <dimension ref="B1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,6 +627,9 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
+      <c r="E8" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -647,9 +650,6 @@
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>61</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed all opcodes to mnemonics to read better
</commit_message>
<xml_diff>
--- a/Documents/Supported Opcodes.xlsx
+++ b/Documents/Supported Opcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\source\repos\David284\CbusTestSuite\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42D94A6-193C-475D-9201-74A223F50DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFE38CD-7B1C-4597-8879-E9AB7FED3D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
   <si>
     <t>WRACK</t>
   </si>
@@ -541,7 +541,7 @@
   <dimension ref="B1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,6 +638,9 @@
       <c r="C9" t="s">
         <v>40</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -712,6 +715,9 @@
       </c>
       <c r="C18" t="s">
         <v>33</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated spreadsheet & comments
</commit_message>
<xml_diff>
--- a/Documents/Supported Opcodes.xlsx
+++ b/Documents/Supported Opcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\source\repos\David284\CbusTestSuite\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59331399-95B5-48B8-9101-4CAA506842D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99FF9E6-3F5A-4D0F-B659-74795680C411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>WRACK</t>
   </si>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,6 +845,9 @@
       <c r="C27" t="s">
         <v>47</v>
       </c>
+      <c r="E27" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
@@ -875,6 +878,9 @@
       <c r="C30" t="s">
         <v>38</v>
       </c>
+      <c r="D30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
@@ -883,6 +889,9 @@
       <c r="C31" t="s">
         <v>12</v>
       </c>
+      <c r="E31" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
@@ -891,6 +900,9 @@
       <c r="C32" t="s">
         <v>51</v>
       </c>
+      <c r="E32" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
@@ -910,6 +922,9 @@
       <c r="C34" t="s">
         <v>19</v>
       </c>
+      <c r="D34" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
@@ -939,6 +954,9 @@
       </c>
       <c r="C37" t="s">
         <v>48</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added NNCLR test & re-arranged sequence
</commit_message>
<xml_diff>
--- a/Documents/Supported Opcodes.xlsx
+++ b/Documents/Supported Opcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\source\repos\David284\CbusTestSuite\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF2FB7C-55FB-4810-AD16-5F4176C0F04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFBD3D3-B556-4A62-9FCA-CAC63AFE803D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
   <si>
     <t>WRACK</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Neumonic</t>
   </si>
   <si>
-    <t>ERR</t>
-  </si>
-  <si>
     <t>Runs bootloader</t>
   </si>
   <si>
@@ -222,12 +219,6 @@
     <t>learn mode</t>
   </si>
   <si>
-    <t>sent by command station</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -235,6 +226,9 @@
   </si>
   <si>
     <t>easy to test from FCU</t>
+  </si>
+  <si>
+    <t>leave learn mode</t>
   </si>
 </sst>
 </file>
@@ -559,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F42"/>
+  <dimension ref="B1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +582,7 @@
         <v>57</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
@@ -599,10 +593,10 @@
         <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -613,10 +607,10 @@
         <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -627,10 +621,10 @@
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -641,10 +635,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -655,13 +649,13 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -672,7 +666,7 @@
         <v>52</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -709,39 +703,39 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>27</v>
+      <c r="B13" s="1">
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>43</v>
@@ -749,65 +743,65 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
-        <v>95</v>
+      <c r="B15" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>56</v>
+      <c r="B16" s="1">
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" t="s">
-        <v>41</v>
+        <v>17</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
-        <v>57</v>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>22</v>
+      <c r="B19" s="1">
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>43</v>
@@ -815,10 +809,13 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>43</v>
@@ -826,21 +823,21 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" t="s">
-        <v>64</v>
+        <v>29</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>43</v>
@@ -848,43 +845,46 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>43</v>
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>67</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" t="s">
-        <v>64</v>
+        <v>25</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>43</v>
@@ -892,10 +892,10 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>43</v>
@@ -903,43 +903,43 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="1">
-        <v>96</v>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" t="s">
-        <v>41</v>
+        <v>12</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>43</v>
@@ -947,10 +947,10 @@
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>43</v>
@@ -958,10 +958,13 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
+        <v>63</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>43</v>
@@ -969,24 +972,21 @@
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
-        <v>14</v>
+      <c r="B35" s="1">
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>43</v>
@@ -994,21 +994,21 @@
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D37" t="s">
         <v>41</v>
@@ -1016,10 +1016,10 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
         <v>41</v>
@@ -1027,51 +1027,40 @@
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>43</v>
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="1">
-        <v>59</v>
-      </c>
-      <c r="C42" t="s">
         <v>0</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E42">
-    <sortCondition ref="C2:C42"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E41">
+    <sortCondition ref="C2:C41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>